<commit_message>
Merged PR 38: Implement demo
Related work items: #365
</commit_message>
<xml_diff>
--- a/DesignerRawData/Excel/TalkerName.xlsx
+++ b/DesignerRawData/Excel/TalkerName.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21629"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67616578-C9F2-4933-8BEA-69E37BBBC95A}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E0CFA3-E773-468F-A918-50BE8A6AA70E}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18720" yWindow="10665" windowWidth="32400" windowHeight="14535" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TalkerName_StringTable" sheetId="1" r:id="rId1"/>
@@ -405,7 +405,7 @@
   <dimension ref="A1:C7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H32" sqref="H32"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>

</xml_diff>